<commit_message>
JavaDoc created & DataProvider added
</commit_message>
<xml_diff>
--- a/src/test/resources/Prod/TrashStore.xlsx
+++ b/src/test/resources/Prod/TrashStore.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arvin\eclipse-workspace\TestNG_Framework\src\test\resources\Prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919E5B89-B298-4791-B80C-9A342AADCDF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFD46F6-ABA2-407E-BB9A-CCFC1114A242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GoogleTrial" sheetId="1" r:id="rId1"/>
+    <sheet name="Google" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>